<commit_message>
fix kern table and Layers_codes.xlsx
</commit_message>
<xml_diff>
--- a/reports/xlsx/Layers_codes.xlsx
+++ b/reports/xlsx/Layers_codes.xlsx
@@ -1,11 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25415"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25629"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="613" documentId="11_924874E5C5FBB6926123EA198B3E8C185103838B" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5FAD93D4-46F2-4844-9E4A-0E41D53BB085}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\for made\Pycharm-projects\Unstructured-field-data-aggregator\reports\xlsx\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83D8B772-1985-4D81-B558-7ED906588337}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -27,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2725" uniqueCount="545">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2725" uniqueCount="546">
   <si>
     <t>system</t>
   </si>
@@ -1662,13 +1667,16 @@
   </si>
   <si>
     <t>Д0Cm</t>
+  </si>
+  <si>
+    <t>C2bch</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1725,9 +1733,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Стандартная">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1765,7 +1773,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Стандартная">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1871,7 +1879,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Стандартная">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2023,29 +2031,29 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P242"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A233" workbookViewId="0">
-      <selection activeCell="B241" sqref="B241:B242"/>
+    <sheetView tabSelected="1" topLeftCell="C85" workbookViewId="0">
+      <selection activeCell="N109" sqref="N109"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.140625" customWidth="1"/>
-    <col min="2" max="2" width="13.140625" customWidth="1"/>
-    <col min="3" max="3" width="13.5703125" customWidth="1"/>
-    <col min="4" max="4" width="16.28515625" customWidth="1"/>
-    <col min="5" max="5" width="11.5703125" customWidth="1"/>
-    <col min="6" max="6" width="11.42578125" customWidth="1"/>
-    <col min="7" max="7" width="11.140625" customWidth="1"/>
-    <col min="8" max="8" width="16.7109375" customWidth="1"/>
-    <col min="9" max="10" width="11.28515625" customWidth="1"/>
+    <col min="1" max="1" width="16.109375" customWidth="1"/>
+    <col min="2" max="2" width="13.109375" customWidth="1"/>
+    <col min="3" max="3" width="13.5546875" customWidth="1"/>
+    <col min="4" max="4" width="16.33203125" customWidth="1"/>
+    <col min="5" max="5" width="11.5546875" customWidth="1"/>
+    <col min="6" max="6" width="11.44140625" customWidth="1"/>
+    <col min="7" max="7" width="11.109375" customWidth="1"/>
+    <col min="8" max="8" width="16.6640625" customWidth="1"/>
+    <col min="9" max="10" width="11.33203125" customWidth="1"/>
     <col min="11" max="12" width="14" customWidth="1"/>
-    <col min="13" max="13" width="14.5703125" customWidth="1"/>
-    <col min="14" max="14" width="16.85546875" customWidth="1"/>
-    <col min="15" max="15" width="11.7109375" customWidth="1"/>
-    <col min="16" max="16" width="14.5703125" customWidth="1"/>
+    <col min="13" max="13" width="14.5546875" customWidth="1"/>
+    <col min="14" max="14" width="16.88671875" customWidth="1"/>
+    <col min="15" max="15" width="11.6640625" customWidth="1"/>
+    <col min="16" max="16" width="14.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2095,7 +2103,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:16" ht="15" customHeight="1">
+    <row r="2" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -2121,7 +2129,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:16">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>16</v>
       </c>
@@ -2147,7 +2155,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:16" ht="15" customHeight="1">
+    <row r="4" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>16</v>
       </c>
@@ -2176,7 +2184,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:16">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>16</v>
       </c>
@@ -2205,7 +2213,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="6" spans="1:16">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>16</v>
       </c>
@@ -2234,7 +2242,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="7" spans="1:16">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>16</v>
       </c>
@@ -2263,7 +2271,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:16">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>16</v>
       </c>
@@ -2292,7 +2300,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="9" spans="1:16">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>16</v>
       </c>
@@ -2321,7 +2329,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="10" spans="1:16">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>16</v>
       </c>
@@ -2350,7 +2358,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="11" spans="1:16">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>16</v>
       </c>
@@ -2379,7 +2387,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="12" spans="1:16">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>16</v>
       </c>
@@ -2408,7 +2416,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="13" spans="1:16">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>16</v>
       </c>
@@ -2434,7 +2442,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="14" spans="1:16">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>16</v>
       </c>
@@ -2460,7 +2468,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="15" spans="1:16">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>46</v>
       </c>
@@ -2489,7 +2497,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="16" spans="1:16">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>46</v>
       </c>
@@ -2518,7 +2526,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="17" spans="1:16">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>46</v>
       </c>
@@ -2547,7 +2555,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="18" spans="1:16">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>46</v>
       </c>
@@ -2573,7 +2581,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="19" spans="1:16">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>46</v>
       </c>
@@ -2596,7 +2604,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="20" spans="1:16" ht="15" customHeight="1">
+    <row r="20" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>61</v>
       </c>
@@ -2625,7 +2633,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="21" spans="1:16">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>61</v>
       </c>
@@ -2654,7 +2662,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="22" spans="1:16">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>61</v>
       </c>
@@ -2683,7 +2691,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="23" spans="1:16">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>61</v>
       </c>
@@ -2712,7 +2720,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="24" spans="1:16">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>61</v>
       </c>
@@ -2741,7 +2749,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="25" spans="1:16">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>61</v>
       </c>
@@ -2770,7 +2778,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="26" spans="1:16">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>61</v>
       </c>
@@ -2799,7 +2807,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="27" spans="1:16">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>87</v>
       </c>
@@ -2825,7 +2833,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="28" spans="1:16">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>87</v>
       </c>
@@ -2851,7 +2859,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="29" spans="1:16">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>87</v>
       </c>
@@ -2877,7 +2885,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="30" spans="1:16">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>87</v>
       </c>
@@ -2903,7 +2911,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="31" spans="1:16">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>87</v>
       </c>
@@ -2929,7 +2937,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="32" spans="1:16">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>106</v>
       </c>
@@ -2953,7 +2961,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="33" spans="1:15">
+    <row r="33" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>106</v>
       </c>
@@ -2977,7 +2985,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="34" spans="1:15">
+    <row r="34" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>106</v>
       </c>
@@ -3001,7 +3009,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="35" spans="1:15">
+    <row r="35" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>106</v>
       </c>
@@ -3025,7 +3033,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="36" spans="1:15">
+    <row r="36" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>106</v>
       </c>
@@ -3049,7 +3057,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="37" spans="1:15">
+    <row r="37" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>106</v>
       </c>
@@ -3073,7 +3081,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="38" spans="1:15">
+    <row r="38" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>106</v>
       </c>
@@ -3097,7 +3105,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="39" spans="1:15">
+    <row r="39" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>106</v>
       </c>
@@ -3121,7 +3129,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="40" spans="1:15">
+    <row r="40" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>106</v>
       </c>
@@ -3144,7 +3152,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="41" spans="1:15">
+    <row r="41" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>106</v>
       </c>
@@ -3167,7 +3175,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="42" spans="1:15">
+    <row r="42" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>106</v>
       </c>
@@ -3190,7 +3198,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="43" spans="1:15">
+    <row r="43" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>106</v>
       </c>
@@ -3213,7 +3221,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="44" spans="1:15" ht="15" customHeight="1">
+    <row r="44" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>106</v>
       </c>
@@ -3245,7 +3253,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="45" spans="1:15">
+    <row r="45" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>106</v>
       </c>
@@ -3277,7 +3285,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="46" spans="1:15">
+    <row r="46" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>106</v>
       </c>
@@ -3309,7 +3317,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="47" spans="1:15">
+    <row r="47" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>106</v>
       </c>
@@ -3341,7 +3349,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="48" spans="1:15">
+    <row r="48" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>106</v>
       </c>
@@ -3373,7 +3381,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="49" spans="1:15">
+    <row r="49" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>106</v>
       </c>
@@ -3405,7 +3413,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="50" spans="1:15">
+    <row r="50" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>106</v>
       </c>
@@ -3437,7 +3445,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="51" spans="1:15">
+    <row r="51" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>106</v>
       </c>
@@ -3469,7 +3477,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="52" spans="1:15">
+    <row r="52" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>106</v>
       </c>
@@ -3501,7 +3509,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="53" spans="1:15" ht="15" customHeight="1">
+    <row r="53" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>106</v>
       </c>
@@ -3536,7 +3544,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="54" spans="1:15">
+    <row r="54" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>106</v>
       </c>
@@ -3571,7 +3579,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="55" spans="1:15">
+    <row r="55" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>106</v>
       </c>
@@ -3606,7 +3614,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="56" spans="1:15">
+    <row r="56" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>106</v>
       </c>
@@ -3641,7 +3649,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="57" spans="1:15">
+    <row r="57" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>106</v>
       </c>
@@ -3676,7 +3684,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="58" spans="1:15">
+    <row r="58" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>106</v>
       </c>
@@ -3711,7 +3719,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="59" spans="1:15">
+    <row r="59" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>106</v>
       </c>
@@ -3746,7 +3754,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="60" spans="1:15" ht="15" customHeight="1">
+    <row r="60" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>106</v>
       </c>
@@ -3778,7 +3786,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="61" spans="1:15">
+    <row r="61" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>106</v>
       </c>
@@ -3810,7 +3818,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="62" spans="1:15">
+    <row r="62" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>106</v>
       </c>
@@ -3842,7 +3850,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="63" spans="1:15">
+    <row r="63" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>106</v>
       </c>
@@ -3874,7 +3882,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="64" spans="1:15">
+    <row r="64" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>106</v>
       </c>
@@ -3906,7 +3914,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="65" spans="1:16">
+    <row r="65" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>106</v>
       </c>
@@ -3938,7 +3946,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="66" spans="1:16">
+    <row r="66" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>106</v>
       </c>
@@ -3970,7 +3978,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="67" spans="1:16">
+    <row r="67" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>106</v>
       </c>
@@ -3999,7 +4007,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="68" spans="1:16">
+    <row r="68" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>106</v>
       </c>
@@ -4028,7 +4036,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="69" spans="1:16">
+    <row r="69" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>106</v>
       </c>
@@ -4060,7 +4068,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="70" spans="1:16">
+    <row r="70" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>106</v>
       </c>
@@ -4092,7 +4100,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="71" spans="1:16">
+    <row r="71" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>106</v>
       </c>
@@ -4121,7 +4129,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="72" spans="1:16">
+    <row r="72" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>204</v>
       </c>
@@ -4147,7 +4155,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="73" spans="1:16">
+    <row r="73" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>204</v>
       </c>
@@ -4179,7 +4187,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="74" spans="1:16">
+    <row r="74" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>204</v>
       </c>
@@ -4211,7 +4219,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="75" spans="1:16">
+    <row r="75" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>204</v>
       </c>
@@ -4243,7 +4251,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="76" spans="1:16">
+    <row r="76" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>204</v>
       </c>
@@ -4275,7 +4283,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="77" spans="1:16">
+    <row r="77" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>204</v>
       </c>
@@ -4307,7 +4315,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="78" spans="1:16">
+    <row r="78" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>204</v>
       </c>
@@ -4339,7 +4347,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="79" spans="1:16">
+    <row r="79" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>204</v>
       </c>
@@ -4371,7 +4379,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="80" spans="1:16">
+    <row r="80" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>204</v>
       </c>
@@ -4412,7 +4420,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="81" spans="1:16">
+    <row r="81" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>204</v>
       </c>
@@ -4453,7 +4461,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="82" spans="1:16">
+    <row r="82" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>204</v>
       </c>
@@ -4494,7 +4502,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="83" spans="1:16">
+    <row r="83" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>204</v>
       </c>
@@ -4535,7 +4543,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="84" spans="1:16">
+    <row r="84" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>204</v>
       </c>
@@ -4576,7 +4584,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="85" spans="1:16">
+    <row r="85" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>204</v>
       </c>
@@ -4617,7 +4625,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="86" spans="1:16">
+    <row r="86" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>204</v>
       </c>
@@ -4658,7 +4666,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="87" spans="1:16">
+    <row r="87" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>204</v>
       </c>
@@ -4699,7 +4707,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="88" spans="1:16">
+    <row r="88" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>204</v>
       </c>
@@ -4740,7 +4748,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="89" spans="1:16">
+    <row r="89" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>204</v>
       </c>
@@ -4781,7 +4789,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="90" spans="1:16">
+    <row r="90" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>204</v>
       </c>
@@ -4822,7 +4830,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="91" spans="1:16">
+    <row r="91" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>204</v>
       </c>
@@ -4863,7 +4871,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="92" spans="1:16">
+    <row r="92" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>204</v>
       </c>
@@ -4904,7 +4912,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="93" spans="1:16">
+    <row r="93" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>204</v>
       </c>
@@ -4945,7 +4953,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="94" spans="1:16">
+    <row r="94" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>204</v>
       </c>
@@ -4986,7 +4994,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="95" spans="1:16">
+    <row r="95" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>204</v>
       </c>
@@ -5027,7 +5035,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="96" spans="1:16">
+    <row r="96" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>204</v>
       </c>
@@ -5068,7 +5076,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="97" spans="1:16">
+    <row r="97" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>204</v>
       </c>
@@ -5109,7 +5117,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="98" spans="1:16">
+    <row r="98" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>204</v>
       </c>
@@ -5150,7 +5158,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="99" spans="1:16">
+    <row r="99" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>204</v>
       </c>
@@ -5191,7 +5199,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="100" spans="1:16">
+    <row r="100" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
         <v>204</v>
       </c>
@@ -5232,7 +5240,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="101" spans="1:16">
+    <row r="101" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
         <v>204</v>
       </c>
@@ -5273,7 +5281,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="102" spans="1:16">
+    <row r="102" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
         <v>204</v>
       </c>
@@ -5314,7 +5322,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="103" spans="1:16">
+    <row r="103" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
         <v>204</v>
       </c>
@@ -5355,7 +5363,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="104" spans="1:16">
+    <row r="104" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
         <v>204</v>
       </c>
@@ -5396,7 +5404,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="105" spans="1:16">
+    <row r="105" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
         <v>204</v>
       </c>
@@ -5437,7 +5445,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="106" spans="1:16">
+    <row r="106" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
         <v>204</v>
       </c>
@@ -5478,7 +5486,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="107" spans="1:16">
+    <row r="107" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
         <v>204</v>
       </c>
@@ -5519,7 +5527,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="108" spans="1:16">
+    <row r="108" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
         <v>204</v>
       </c>
@@ -5560,7 +5568,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="109" spans="1:16">
+    <row r="109" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
         <v>204</v>
       </c>
@@ -5586,7 +5594,7 @@
         <v>50</v>
       </c>
       <c r="N109" t="s">
-        <v>273</v>
+        <v>545</v>
       </c>
       <c r="O109" t="s">
         <v>275</v>
@@ -5595,7 +5603,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="110" spans="1:16">
+    <row r="110" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
         <v>204</v>
       </c>
@@ -5621,7 +5629,7 @@
         <v>50</v>
       </c>
       <c r="N110" t="s">
-        <v>273</v>
+        <v>545</v>
       </c>
       <c r="O110" t="s">
         <v>275</v>
@@ -5630,7 +5638,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="111" spans="1:16">
+    <row r="111" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
         <v>204</v>
       </c>
@@ -5656,7 +5664,7 @@
         <v>50</v>
       </c>
       <c r="N111" t="s">
-        <v>273</v>
+        <v>545</v>
       </c>
       <c r="O111" t="s">
         <v>275</v>
@@ -5665,7 +5673,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="112" spans="1:16">
+    <row r="112" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
         <v>204</v>
       </c>
@@ -5691,7 +5699,7 @@
         <v>50</v>
       </c>
       <c r="N112" t="s">
-        <v>273</v>
+        <v>545</v>
       </c>
       <c r="O112" t="s">
         <v>275</v>
@@ -5700,7 +5708,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="113" spans="1:16">
+    <row r="113" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
         <v>204</v>
       </c>
@@ -5726,7 +5734,7 @@
         <v>50</v>
       </c>
       <c r="N113" t="s">
-        <v>273</v>
+        <v>545</v>
       </c>
       <c r="O113" t="s">
         <v>275</v>
@@ -5735,7 +5743,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="114" spans="1:16">
+    <row r="114" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
         <v>204</v>
       </c>
@@ -5761,7 +5769,7 @@
         <v>50</v>
       </c>
       <c r="N114" t="s">
-        <v>273</v>
+        <v>545</v>
       </c>
       <c r="O114" t="s">
         <v>275</v>
@@ -5770,7 +5778,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="115" spans="1:16">
+    <row r="115" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
         <v>204</v>
       </c>
@@ -5808,7 +5816,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="116" spans="1:16">
+    <row r="116" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
         <v>204</v>
       </c>
@@ -5846,7 +5854,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="117" spans="1:16">
+    <row r="117" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
         <v>204</v>
       </c>
@@ -5884,7 +5892,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="118" spans="1:16">
+    <row r="118" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
         <v>204</v>
       </c>
@@ -5922,7 +5930,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="119" spans="1:16">
+    <row r="119" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
         <v>204</v>
       </c>
@@ -5960,7 +5968,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="120" spans="1:16">
+    <row r="120" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
         <v>204</v>
       </c>
@@ -5998,7 +6006,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="121" spans="1:16">
+    <row r="121" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
         <v>204</v>
       </c>
@@ -6036,7 +6044,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="122" spans="1:16">
+    <row r="122" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
         <v>204</v>
       </c>
@@ -6074,7 +6082,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="123" spans="1:16">
+    <row r="123" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
         <v>204</v>
       </c>
@@ -6112,7 +6120,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="124" spans="1:16">
+    <row r="124" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
         <v>204</v>
       </c>
@@ -6150,7 +6158,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="125" spans="1:16">
+    <row r="125" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
         <v>204</v>
       </c>
@@ -6188,7 +6196,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="126" spans="1:16">
+    <row r="126" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
         <v>204</v>
       </c>
@@ -6226,7 +6234,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="127" spans="1:16">
+    <row r="127" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
         <v>204</v>
       </c>
@@ -6264,7 +6272,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="128" spans="1:16">
+    <row r="128" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
         <v>204</v>
       </c>
@@ -6302,7 +6310,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="129" spans="1:16">
+    <row r="129" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
         <v>204</v>
       </c>
@@ -6340,7 +6348,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="130" spans="1:16">
+    <row r="130" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
         <v>204</v>
       </c>
@@ -6378,7 +6386,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="131" spans="1:16">
+    <row r="131" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
         <v>204</v>
       </c>
@@ -6416,7 +6424,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="132" spans="1:16">
+    <row r="132" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
         <v>204</v>
       </c>
@@ -6454,7 +6462,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="133" spans="1:16">
+    <row r="133" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
         <v>204</v>
       </c>
@@ -6492,7 +6500,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="134" spans="1:16">
+    <row r="134" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
         <v>204</v>
       </c>
@@ -6530,7 +6538,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="135" spans="1:16">
+    <row r="135" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
         <v>204</v>
       </c>
@@ -6568,7 +6576,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="136" spans="1:16">
+    <row r="136" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
         <v>204</v>
       </c>
@@ -6606,7 +6614,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="137" spans="1:16">
+    <row r="137" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
         <v>204</v>
       </c>
@@ -6644,7 +6652,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="138" spans="1:16">
+    <row r="138" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
         <v>204</v>
       </c>
@@ -6682,7 +6690,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="139" spans="1:16">
+    <row r="139" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
         <v>204</v>
       </c>
@@ -6720,7 +6728,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="140" spans="1:16">
+    <row r="140" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
         <v>204</v>
       </c>
@@ -6758,7 +6766,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="141" spans="1:16">
+    <row r="141" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
         <v>204</v>
       </c>
@@ -6796,7 +6804,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="142" spans="1:16">
+    <row r="142" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
         <v>204</v>
       </c>
@@ -6834,7 +6842,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="143" spans="1:16">
+    <row r="143" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
         <v>204</v>
       </c>
@@ -6872,7 +6880,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="144" spans="1:16">
+    <row r="144" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
         <v>204</v>
       </c>
@@ -6910,7 +6918,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="145" spans="1:16">
+    <row r="145" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
         <v>204</v>
       </c>
@@ -6948,7 +6956,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="146" spans="1:16">
+    <row r="146" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
         <v>204</v>
       </c>
@@ -6986,7 +6994,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="147" spans="1:16">
+    <row r="147" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
         <v>204</v>
       </c>
@@ -7024,7 +7032,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="148" spans="1:16">
+    <row r="148" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
         <v>204</v>
       </c>
@@ -7062,7 +7070,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="149" spans="1:16">
+    <row r="149" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
         <v>204</v>
       </c>
@@ -7100,7 +7108,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="150" spans="1:16">
+    <row r="150" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A150" t="s">
         <v>204</v>
       </c>
@@ -7138,7 +7146,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="151" spans="1:16">
+    <row r="151" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
         <v>204</v>
       </c>
@@ -7176,7 +7184,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="152" spans="1:16">
+    <row r="152" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A152" t="s">
         <v>204</v>
       </c>
@@ -7214,7 +7222,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="153" spans="1:16">
+    <row r="153" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A153" t="s">
         <v>204</v>
       </c>
@@ -7252,7 +7260,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="154" spans="1:16">
+    <row r="154" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A154" t="s">
         <v>204</v>
       </c>
@@ -7290,7 +7298,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="155" spans="1:16">
+    <row r="155" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A155" t="s">
         <v>204</v>
       </c>
@@ -7328,7 +7336,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="156" spans="1:16">
+    <row r="156" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A156" t="s">
         <v>204</v>
       </c>
@@ -7366,7 +7374,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="157" spans="1:16">
+    <row r="157" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A157" t="s">
         <v>204</v>
       </c>
@@ -7404,7 +7412,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="158" spans="1:16">
+    <row r="158" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A158" t="s">
         <v>204</v>
       </c>
@@ -7442,7 +7450,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="159" spans="1:16">
+    <row r="159" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A159" t="s">
         <v>204</v>
       </c>
@@ -7480,7 +7488,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="160" spans="1:16">
+    <row r="160" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A160" t="s">
         <v>204</v>
       </c>
@@ -7518,7 +7526,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="161" spans="1:16">
+    <row r="161" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A161" t="s">
         <v>204</v>
       </c>
@@ -7556,7 +7564,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="162" spans="1:16">
+    <row r="162" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A162" t="s">
         <v>204</v>
       </c>
@@ -7594,7 +7602,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="163" spans="1:16">
+    <row r="163" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A163" t="s">
         <v>204</v>
       </c>
@@ -7632,7 +7640,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="164" spans="1:16">
+    <row r="164" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A164" t="s">
         <v>384</v>
       </c>
@@ -7673,7 +7681,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="165" spans="1:16">
+    <row r="165" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A165" t="s">
         <v>384</v>
       </c>
@@ -7714,7 +7722,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="166" spans="1:16">
+    <row r="166" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A166" t="s">
         <v>384</v>
       </c>
@@ -7755,7 +7763,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="167" spans="1:16">
+    <row r="167" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A167" t="s">
         <v>384</v>
       </c>
@@ -7796,7 +7804,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="168" spans="1:16">
+    <row r="168" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A168" t="s">
         <v>384</v>
       </c>
@@ -7837,7 +7845,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="169" spans="1:16">
+    <row r="169" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A169" t="s">
         <v>384</v>
       </c>
@@ -7878,7 +7886,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="170" spans="1:16">
+    <row r="170" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A170" t="s">
         <v>384</v>
       </c>
@@ -7919,7 +7927,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="171" spans="1:16">
+    <row r="171" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A171" t="s">
         <v>384</v>
       </c>
@@ -7960,7 +7968,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="172" spans="1:16">
+    <row r="172" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A172" t="s">
         <v>384</v>
       </c>
@@ -8001,7 +8009,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="173" spans="1:16">
+    <row r="173" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A173" t="s">
         <v>384</v>
       </c>
@@ -8042,7 +8050,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="174" spans="1:16">
+    <row r="174" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A174" t="s">
         <v>384</v>
       </c>
@@ -8083,7 +8091,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="175" spans="1:16">
+    <row r="175" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A175" t="s">
         <v>384</v>
       </c>
@@ -8124,7 +8132,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="176" spans="1:16">
+    <row r="176" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A176" t="s">
         <v>384</v>
       </c>
@@ -8165,7 +8173,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="177" spans="1:16">
+    <row r="177" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A177" t="s">
         <v>384</v>
       </c>
@@ -8206,7 +8214,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="178" spans="1:16">
+    <row r="178" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A178" t="s">
         <v>384</v>
       </c>
@@ -8247,7 +8255,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="179" spans="1:16">
+    <row r="179" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A179" t="s">
         <v>384</v>
       </c>
@@ -8288,7 +8296,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="180" spans="1:16">
+    <row r="180" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A180" t="s">
         <v>384</v>
       </c>
@@ -8329,7 +8337,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="181" spans="1:16">
+    <row r="181" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A181" t="s">
         <v>384</v>
       </c>
@@ -8370,7 +8378,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="182" spans="1:16">
+    <row r="182" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A182" t="s">
         <v>384</v>
       </c>
@@ -8411,7 +8419,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="183" spans="1:16">
+    <row r="183" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A183" t="s">
         <v>384</v>
       </c>
@@ -8452,7 +8460,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="184" spans="1:16">
+    <row r="184" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A184" t="s">
         <v>384</v>
       </c>
@@ -8493,7 +8501,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="185" spans="1:16">
+    <row r="185" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A185" t="s">
         <v>384</v>
       </c>
@@ -8534,7 +8542,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="186" spans="1:16">
+    <row r="186" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A186" t="s">
         <v>384</v>
       </c>
@@ -8575,7 +8583,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="187" spans="1:16">
+    <row r="187" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A187" t="s">
         <v>384</v>
       </c>
@@ -8616,7 +8624,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="188" spans="1:16">
+    <row r="188" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A188" t="s">
         <v>384</v>
       </c>
@@ -8657,7 +8665,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="189" spans="1:16">
+    <row r="189" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A189" t="s">
         <v>384</v>
       </c>
@@ -8698,7 +8706,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="190" spans="1:16">
+    <row r="190" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A190" t="s">
         <v>384</v>
       </c>
@@ -8739,7 +8747,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="191" spans="1:16">
+    <row r="191" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A191" t="s">
         <v>384</v>
       </c>
@@ -8780,7 +8788,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="192" spans="1:16">
+    <row r="192" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A192" t="s">
         <v>384</v>
       </c>
@@ -8821,7 +8829,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="193" spans="1:16">
+    <row r="193" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A193" t="s">
         <v>384</v>
       </c>
@@ -8862,7 +8870,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="194" spans="1:16">
+    <row r="194" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A194" t="s">
         <v>384</v>
       </c>
@@ -8903,7 +8911,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="195" spans="1:16">
+    <row r="195" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A195" t="s">
         <v>384</v>
       </c>
@@ -8944,7 +8952,7 @@
         <v>448</v>
       </c>
     </row>
-    <row r="196" spans="1:16">
+    <row r="196" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A196" t="s">
         <v>384</v>
       </c>
@@ -8985,7 +8993,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="197" spans="1:16">
+    <row r="197" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A197" t="s">
         <v>384</v>
       </c>
@@ -9026,7 +9034,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="198" spans="1:16">
+    <row r="198" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A198" t="s">
         <v>384</v>
       </c>
@@ -9067,7 +9075,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="199" spans="1:16">
+    <row r="199" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A199" t="s">
         <v>384</v>
       </c>
@@ -9108,7 +9116,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="200" spans="1:16">
+    <row r="200" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A200" t="s">
         <v>384</v>
       </c>
@@ -9149,7 +9157,7 @@
         <v>459</v>
       </c>
     </row>
-    <row r="201" spans="1:16">
+    <row r="201" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A201" t="s">
         <v>384</v>
       </c>
@@ -9190,7 +9198,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="202" spans="1:16">
+    <row r="202" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A202" t="s">
         <v>384</v>
       </c>
@@ -9231,7 +9239,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="203" spans="1:16">
+    <row r="203" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A203" t="s">
         <v>384</v>
       </c>
@@ -9272,7 +9280,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="204" spans="1:16">
+    <row r="204" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A204" t="s">
         <v>384</v>
       </c>
@@ -9313,7 +9321,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="205" spans="1:16">
+    <row r="205" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A205" t="s">
         <v>384</v>
       </c>
@@ -9354,7 +9362,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="206" spans="1:16">
+    <row r="206" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A206" t="s">
         <v>384</v>
       </c>
@@ -9395,7 +9403,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="207" spans="1:16">
+    <row r="207" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A207" t="s">
         <v>384</v>
       </c>
@@ -9436,7 +9444,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="208" spans="1:16">
+    <row r="208" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A208" t="s">
         <v>384</v>
       </c>
@@ -9477,7 +9485,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="209" spans="1:16">
+    <row r="209" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A209" t="s">
         <v>384</v>
       </c>
@@ -9518,7 +9526,7 @@
         <v>474</v>
       </c>
     </row>
-    <row r="210" spans="1:16">
+    <row r="210" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A210" t="s">
         <v>384</v>
       </c>
@@ -9559,7 +9567,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="211" spans="1:16">
+    <row r="211" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A211" t="s">
         <v>384</v>
       </c>
@@ -9600,7 +9608,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="212" spans="1:16">
+    <row r="212" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A212" t="s">
         <v>384</v>
       </c>
@@ -9641,7 +9649,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="213" spans="1:16">
+    <row r="213" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A213" t="s">
         <v>384</v>
       </c>
@@ -9682,7 +9690,7 @@
         <v>481</v>
       </c>
     </row>
-    <row r="214" spans="1:16">
+    <row r="214" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A214" t="s">
         <v>384</v>
       </c>
@@ -9723,7 +9731,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="215" spans="1:16">
+    <row r="215" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A215" t="s">
         <v>384</v>
       </c>
@@ -9764,7 +9772,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="216" spans="1:16">
+    <row r="216" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A216" t="s">
         <v>384</v>
       </c>
@@ -9805,7 +9813,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="217" spans="1:16">
+    <row r="217" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A217" t="s">
         <v>384</v>
       </c>
@@ -9846,7 +9854,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="218" spans="1:16">
+    <row r="218" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A218" t="s">
         <v>384</v>
       </c>
@@ -9887,7 +9895,7 @@
         <v>486</v>
       </c>
     </row>
-    <row r="219" spans="1:16">
+    <row r="219" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A219" t="s">
         <v>384</v>
       </c>
@@ -9928,7 +9936,7 @@
         <v>487</v>
       </c>
     </row>
-    <row r="220" spans="1:16">
+    <row r="220" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A220" t="s">
         <v>384</v>
       </c>
@@ -9969,7 +9977,7 @@
         <v>488</v>
       </c>
     </row>
-    <row r="221" spans="1:16">
+    <row r="221" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A221" t="s">
         <v>384</v>
       </c>
@@ -10010,7 +10018,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="222" spans="1:16">
+    <row r="222" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A222" t="s">
         <v>384</v>
       </c>
@@ -10051,7 +10059,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="223" spans="1:16">
+    <row r="223" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A223" t="s">
         <v>384</v>
       </c>
@@ -10092,7 +10100,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="224" spans="1:16">
+    <row r="224" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A224" t="s">
         <v>384</v>
       </c>
@@ -10133,7 +10141,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="225" spans="1:16">
+    <row r="225" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A225" t="s">
         <v>384</v>
       </c>
@@ -10174,7 +10182,7 @@
         <v>493</v>
       </c>
     </row>
-    <row r="226" spans="1:16">
+    <row r="226" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A226" t="s">
         <v>384</v>
       </c>
@@ -10215,7 +10223,7 @@
         <v>494</v>
       </c>
     </row>
-    <row r="227" spans="1:16">
+    <row r="227" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A227" t="s">
         <v>384</v>
       </c>
@@ -10256,7 +10264,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="228" spans="1:16">
+    <row r="228" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A228" t="s">
         <v>384</v>
       </c>
@@ -10297,7 +10305,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="229" spans="1:16">
+    <row r="229" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A229" t="s">
         <v>384</v>
       </c>
@@ -10335,7 +10343,7 @@
         <v>505</v>
       </c>
     </row>
-    <row r="230" spans="1:16">
+    <row r="230" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A230" t="s">
         <v>384</v>
       </c>
@@ -10373,7 +10381,7 @@
         <v>506</v>
       </c>
     </row>
-    <row r="231" spans="1:16">
+    <row r="231" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A231" t="s">
         <v>384</v>
       </c>
@@ -10411,7 +10419,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="232" spans="1:16">
+    <row r="232" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A232" t="s">
         <v>384</v>
       </c>
@@ -10449,7 +10457,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="233" spans="1:16">
+    <row r="233" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A233" t="s">
         <v>384</v>
       </c>
@@ -10487,7 +10495,7 @@
         <v>515</v>
       </c>
     </row>
-    <row r="234" spans="1:16">
+    <row r="234" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A234" t="s">
         <v>384</v>
       </c>
@@ -10525,7 +10533,7 @@
         <v>516</v>
       </c>
     </row>
-    <row r="235" spans="1:16">
+    <row r="235" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A235" t="s">
         <v>384</v>
       </c>
@@ -10560,7 +10568,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="236" spans="1:16">
+    <row r="236" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A236" t="s">
         <v>522</v>
       </c>
@@ -10586,7 +10594,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="237" spans="1:16">
+    <row r="237" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A237" t="s">
         <v>522</v>
       </c>
@@ -10612,7 +10620,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="238" spans="1:16">
+    <row r="238" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A238" t="s">
         <v>530</v>
       </c>
@@ -10638,7 +10646,7 @@
         <v>534</v>
       </c>
     </row>
-    <row r="239" spans="1:16">
+    <row r="239" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A239" t="s">
         <v>530</v>
       </c>
@@ -10661,7 +10669,7 @@
         <v>537</v>
       </c>
     </row>
-    <row r="240" spans="1:16">
+    <row r="240" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A240" t="s">
         <v>530</v>
       </c>
@@ -10684,7 +10692,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="241" spans="2:15">
+    <row r="241" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B241" t="s">
         <v>540</v>
       </c>
@@ -10698,7 +10706,7 @@
         <v>543</v>
       </c>
     </row>
-    <row r="242" spans="2:15">
+    <row r="242" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B242" t="s">
         <v>540</v>
       </c>

</xml_diff>